<commit_message>
opdater Epinion og tilføj Voxmeter (29.4)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t xml:space="preserve">http://nyheder.tv2.dk/politik/2017-09-28-liberal-alliance-gaar-tilbage-i-ny-maaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.dr.dk/nyheder/politik/maaling-roed-bloks-forspring-skrumper-gevaldigt</t>
   </si>
   <si>
     <t xml:space="preserve">http://nyheder.tv2.dk/politik/2017-10-26-blaa-blok-gaar-markant-frem-i-ny-maaling-solid-roed-foering-er-vaek</t>
@@ -58916,44 +58919,46 @@
         <v>10</v>
       </c>
       <c r="E1127" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F1127" t="n">
-        <v>29.7</v>
+        <v>26.6</v>
       </c>
       <c r="G1127" t="n">
-        <v>4.2</v>
+        <v>5.4</v>
       </c>
       <c r="H1127" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="I1127" t="n">
-        <v>1.6</v>
+        <v>2.3</v>
       </c>
       <c r="J1127" t="n">
+        <v>4</v>
+      </c>
+      <c r="K1127" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="L1127" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M1127" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="N1127" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="O1127" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="P1127" t="n">
         <v>4.8</v>
       </c>
-      <c r="K1127" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="L1127"/>
-      <c r="M1127" t="n">
-        <v>18.2</v>
-      </c>
-      <c r="N1127" t="n">
-        <v>17.7</v>
-      </c>
-      <c r="O1127" t="n">
-        <v>9.2</v>
-      </c>
-      <c r="P1127" t="n">
-        <v>4.7</v>
-      </c>
       <c r="Q1127" t="n">
-        <v>1563</v>
+        <v>1643</v>
       </c>
       <c r="R1127" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1128">
@@ -59065,7 +59070,63 @@
         <v>1017</v>
       </c>
       <c r="R1129" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="n">
+        <v>1129</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1130" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1130" t="n">
+        <v>10</v>
+      </c>
+      <c r="E1130" t="n">
+        <v>29</v>
+      </c>
+      <c r="F1130" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="G1130" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H1130" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="I1130" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J1130" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="K1130" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="L1130" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M1130" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="N1130" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="O1130" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="P1130" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="Q1130" t="n">
+        <v>1049</v>
+      </c>
+      <c r="R1130" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tilføj Gallup (9.11) og Voxmeter (11.11)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.altinget.dk/artikel/maaling-blaa-blok-haler-ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://voxmeter.dk/index.php/meningsmalinger/#</t>
   </si>
 </sst>
 </file>
@@ -59242,6 +59245,118 @@
         <v>89</v>
       </c>
     </row>
+    <row r="1133">
+      <c r="A1133" t="n">
+        <v>1132</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1133" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1133" t="n">
+        <v>11</v>
+      </c>
+      <c r="E1133" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1133" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="G1133" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H1133" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="I1133" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J1133" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="K1133" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="L1133" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M1133" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="N1133" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="O1133" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="P1133" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="Q1133" t="n">
+        <v>1507</v>
+      </c>
+      <c r="R1133" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="n">
+        <v>1133</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1134" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1134" t="n">
+        <v>11</v>
+      </c>
+      <c r="E1134" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1134" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="G1134" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="H1134" t="n">
+        <v>5</v>
+      </c>
+      <c r="I1134" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J1134" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K1134" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="L1134" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M1134" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="N1134" t="n">
+        <v>19.6</v>
+      </c>
+      <c r="O1134" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="P1134" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="Q1134" t="n">
+        <v>1030</v>
+      </c>
+      <c r="R1134" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
update datasets and figures
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -321,9 +321,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.altinget.dk/artikel/maaling-blaa-blok-haler-ind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://voxmeter.dk/index.php/meningsmalinger/#</t>
   </si>
 </sst>
 </file>
@@ -59354,7 +59351,63 @@
         <v>1030</v>
       </c>
       <c r="R1134" t="s">
-        <v>103</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="n">
+        <v>1134</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1135" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1135" t="n">
+        <v>11</v>
+      </c>
+      <c r="E1135" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1135" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="G1135" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="H1135" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I1135" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J1135" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="K1135" t="n">
+        <v>5</v>
+      </c>
+      <c r="L1135" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M1135" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="N1135" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="O1135" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="P1135" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="Q1135" t="n">
+        <v>1025</v>
+      </c>
+      <c r="R1135" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tilføj Norstat (19.11) og Voxmeter (26.11)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.altinget.dk/artikel/maaling-blaa-blok-haler-ind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.altinget.dk/artikel/maaling-blaa-blok-taber-igen-terraen</t>
   </si>
 </sst>
 </file>
@@ -59410,6 +59413,116 @@
         <v>89</v>
       </c>
     </row>
+    <row r="1136">
+      <c r="A1136" t="n">
+        <v>1135</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1136" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1136" t="n">
+        <v>11</v>
+      </c>
+      <c r="E1136" t="n">
+        <v>19</v>
+      </c>
+      <c r="F1136" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="G1136" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="H1136" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="I1136" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J1136" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="K1136" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="L1136"/>
+      <c r="M1136" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="N1136" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="O1136" t="n">
+        <v>8</v>
+      </c>
+      <c r="P1136" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q1136" t="n">
+        <v>1573</v>
+      </c>
+      <c r="R1136" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="n">
+        <v>1136</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1137" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1137" t="n">
+        <v>11</v>
+      </c>
+      <c r="E1137" t="n">
+        <v>26</v>
+      </c>
+      <c r="F1137" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="G1137" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="H1137" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="I1137" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1137" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="K1137" t="n">
+        <v>6</v>
+      </c>
+      <c r="L1137" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M1137" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="N1137" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="O1137" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="P1137" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="Q1137" t="n">
+        <v>1019</v>
+      </c>
+      <c r="R1137" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Greens (30.11) og Epinion (1.12)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t xml:space="preserve">http://nyheder.tv2.dk/politik/2017-11-30-ny-maaling-kommunalvalgssejr-smitter-af-paa-mette-frederiksen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.dr.dk/nyheder/politik/maaling-dansk-folkeparti-taber-terraen-s-i-medvind</t>
   </si>
 </sst>
 </file>
@@ -59582,6 +59585,118 @@
         <v>104</v>
       </c>
     </row>
+    <row r="1139">
+      <c r="A1139" t="n">
+        <v>1138</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1139" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1139" t="n">
+        <v>11</v>
+      </c>
+      <c r="E1139" t="n">
+        <v>30</v>
+      </c>
+      <c r="F1139" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="G1139" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="H1139" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="I1139" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J1139" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K1139" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="L1139" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M1139" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="N1139" t="n">
+        <v>19.7</v>
+      </c>
+      <c r="O1139" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="P1139" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="Q1139" t="n">
+        <v>1262</v>
+      </c>
+      <c r="R1139" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="n">
+        <v>1139</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1140" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1140" t="n">
+        <v>12</v>
+      </c>
+      <c r="E1140" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1140" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="G1140" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="H1140" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="I1140" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J1140" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="K1140" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L1140" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M1140" t="n">
+        <v>16</v>
+      </c>
+      <c r="N1140" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="O1140" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="P1140" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="Q1140" t="n">
+        <v>1737</v>
+      </c>
+      <c r="R1140" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Gallup (7.12) og Voxmeter (9.12)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -59753,6 +59753,118 @@
         <v>89</v>
       </c>
     </row>
+    <row r="1142">
+      <c r="A1142" t="n">
+        <v>1141</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1142" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1142" t="n">
+        <v>12</v>
+      </c>
+      <c r="E1142" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1142" t="n">
+        <v>29</v>
+      </c>
+      <c r="G1142" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="H1142" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="I1142" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J1142" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="K1142" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="L1142" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M1142" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="N1142" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="O1142" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="P1142" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="Q1142" t="n">
+        <v>1497</v>
+      </c>
+      <c r="R1142" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="n">
+        <v>1142</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1143" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1143" t="n">
+        <v>12</v>
+      </c>
+      <c r="E1143" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1143" t="n">
+        <v>27.8</v>
+      </c>
+      <c r="G1143" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="H1143" t="n">
+        <v>4</v>
+      </c>
+      <c r="I1143" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J1143" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="K1143" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="L1143" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1143" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="N1143" t="n">
+        <v>19.1</v>
+      </c>
+      <c r="O1143" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="P1143" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="Q1143" t="n">
+        <v>1019</v>
+      </c>
+      <c r="R1143" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
opdater figurer og data
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -59921,6 +59921,174 @@
         <v>86</v>
       </c>
     </row>
+    <row r="1145">
+      <c r="A1145" t="n">
+        <v>1144</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1145" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1145" t="n">
+        <v>11</v>
+      </c>
+      <c r="E1145" t="n">
+        <v>13</v>
+      </c>
+      <c r="F1145" t="n">
+        <v>24.6</v>
+      </c>
+      <c r="G1145" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H1145" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="I1145" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="J1145" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K1145" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="L1145" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M1145" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="N1145" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="O1145" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="P1145" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="Q1145" t="n">
+        <v>1598</v>
+      </c>
+      <c r="R1145" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="n">
+        <v>1145</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1146" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1146" t="n">
+        <v>12</v>
+      </c>
+      <c r="E1146" t="n">
+        <v>10</v>
+      </c>
+      <c r="F1146" t="n">
+        <v>29</v>
+      </c>
+      <c r="G1146" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="H1146" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="I1146" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J1146" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="K1146" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="L1146" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M1146" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="N1146" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="O1146" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="P1146" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="Q1146" t="n">
+        <v>1602</v>
+      </c>
+      <c r="R1146" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="n">
+        <v>1146</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1147" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D1147" t="n">
+        <v>12</v>
+      </c>
+      <c r="E1147" t="n">
+        <v>17</v>
+      </c>
+      <c r="F1147" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="G1147" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H1147" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="I1147" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J1147" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="K1147" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="L1147" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M1147" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="N1147" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="O1147" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="P1147" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="Q1147" t="n">
+        <v>1019</v>
+      </c>
+      <c r="R1147" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Voxmeter (7.1) og YouGov (7.1)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -60207,6 +60207,118 @@
         <v>107</v>
       </c>
     </row>
+    <row r="1150">
+      <c r="A1150" t="n">
+        <v>1149</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1150" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1150" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1150" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1150" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="G1150" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="H1150" t="n">
+        <v>4</v>
+      </c>
+      <c r="I1150" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J1150" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K1150" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="L1150" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M1150" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="N1150" t="n">
+        <v>19.1</v>
+      </c>
+      <c r="O1150" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="P1150" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="Q1150" t="n">
+        <v>1035</v>
+      </c>
+      <c r="R1150" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="n">
+        <v>1150</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1151" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1151" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1151" t="n">
+        <v>7</v>
+      </c>
+      <c r="F1151" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="G1151" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H1151" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="I1151" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="J1151" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="K1151" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="L1151" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M1151" t="n">
+        <v>17</v>
+      </c>
+      <c r="N1151" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="O1151" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="P1151" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="Q1151" t="n">
+        <v>1410</v>
+      </c>
+      <c r="R1151" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj YouGov (22.1) og Voxmeter (28.1)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -60549,6 +60549,118 @@
         <v>109</v>
       </c>
     </row>
+    <row r="1156">
+      <c r="A1156" t="n">
+        <v>1155</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1156" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1156" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1156" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1156" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="G1156" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="H1156" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="I1156" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="J1156" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="K1156" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="L1156" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M1156" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="N1156" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="O1156" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="P1156" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="Q1156" t="n">
+        <v>1460</v>
+      </c>
+      <c r="R1156" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="n">
+        <v>1156</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1157" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1157" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1157" t="n">
+        <v>28</v>
+      </c>
+      <c r="F1157" t="n">
+        <v>28.9</v>
+      </c>
+      <c r="G1157" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="H1157" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="I1157" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J1157" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="K1157" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="L1157" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M1157" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="N1157" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="O1157" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="P1157" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="Q1157" t="n">
+        <v>1017</v>
+      </c>
+      <c r="R1157" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Epinion (14.2) og Voxmeter (18.2)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.altinget.dk/artikel/ny-maaling-roed-blok-udbygger-foering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.dr.dk/nyheder/politik/maaling-hvis-kvinderne-bestemte-var-danmark-roedt</t>
   </si>
 </sst>
 </file>
@@ -60942,6 +60945,118 @@
         <v>86</v>
       </c>
     </row>
+    <row r="1163">
+      <c r="A1163" t="n">
+        <v>1162</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1163" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1163" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1163" t="n">
+        <v>14</v>
+      </c>
+      <c r="F1163" t="n">
+        <v>28</v>
+      </c>
+      <c r="G1163" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="H1163" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I1163" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J1163" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="K1163" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="L1163" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M1163" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="N1163" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="O1163" t="n">
+        <v>8</v>
+      </c>
+      <c r="P1163" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="Q1163" t="n">
+        <v>1573</v>
+      </c>
+      <c r="R1163" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="n">
+        <v>1163</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1164" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1164" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1164" t="n">
+        <v>18</v>
+      </c>
+      <c r="F1164" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="G1164" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1164" t="n">
+        <v>4</v>
+      </c>
+      <c r="I1164" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J1164" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K1164" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="L1164" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M1164" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="N1164" t="n">
+        <v>20</v>
+      </c>
+      <c r="O1164" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="P1164" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="Q1164" t="n">
+        <v>1026</v>
+      </c>
+      <c r="R1164" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Gallup (8.3) og Voxmeter (11.3)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -61228,6 +61228,118 @@
         <v>89</v>
       </c>
     </row>
+    <row r="1168">
+      <c r="A1168" t="n">
+        <v>1167</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1168" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1168" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1168" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1168" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="G1168" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="H1168" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="I1168" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J1168" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="K1168" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="L1168" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M1168" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="N1168" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="O1168" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="P1168" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="Q1168" t="n">
+        <v>1590</v>
+      </c>
+      <c r="R1168" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="n">
+        <v>1168</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1169" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1169" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1169" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1169" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="G1169" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H1169" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I1169" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J1169" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="K1169" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="L1169" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M1169" t="n">
+        <v>18</v>
+      </c>
+      <c r="N1169" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="O1169" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="P1169" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="Q1169" t="n">
+        <v>1043</v>
+      </c>
+      <c r="R1169" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Norstat (20.3) og Megafon (22.3)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -352,6 +352,12 @@
   <si>
     <t xml:space="preserve">http://nyheder.tv2.dk/politik/2018-02-22-alternativet-har-mistet-to-tredjedele-af-deres-vaelgere-paa-to-aar-viser-ny</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://www.altinget.dk/artikel/ny-maaling-mette-frederiksen-er-slaaet-tilbage-til-start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nyheder.tv2.dk/politik/2018-03-22-ny-maaling-dansk-folkeparti-ligger-fortsat-langt-fra-valgresultatet</t>
+  </si>
 </sst>
 </file>
 
@@ -61396,6 +61402,118 @@
         <v>89</v>
       </c>
     </row>
+    <row r="1171">
+      <c r="A1171" t="n">
+        <v>1170</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1171" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1171" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1171" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1171" t="n">
+        <v>25</v>
+      </c>
+      <c r="G1171" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="H1171" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="I1171" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J1171" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="K1171" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="L1171" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M1171" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="N1171" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="O1171" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="P1171" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="Q1171" t="n">
+        <v>1501</v>
+      </c>
+      <c r="R1171" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="n">
+        <v>1171</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1172" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1172" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1172" t="n">
+        <v>22</v>
+      </c>
+      <c r="F1172" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="G1172" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="H1172" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="I1172" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J1172" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="K1172" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="L1172" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M1172" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="N1172" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="O1172" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="P1172" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="Q1172" t="n">
+        <v>1022</v>
+      </c>
+      <c r="R1172" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Norstat (23.5) og Voxmeter (27.5)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -62478,6 +62478,118 @@
         <v>118</v>
       </c>
     </row>
+    <row r="1190">
+      <c r="A1190" t="n">
+        <v>1189</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1190" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1190" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1190" t="n">
+        <v>23</v>
+      </c>
+      <c r="F1190" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="G1190" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H1190" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="I1190" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J1190" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="K1190" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L1190" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M1190" t="n">
+        <v>17</v>
+      </c>
+      <c r="N1190" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="O1190" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="P1190" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="Q1190" t="n">
+        <v>1210</v>
+      </c>
+      <c r="R1190" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="n">
+        <v>1190</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1191" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1191" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1191" t="n">
+        <v>27</v>
+      </c>
+      <c r="F1191" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="G1191" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="H1191" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I1191" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1191" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="K1191" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="L1191" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M1191" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="N1191" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="O1191" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="P1191" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="Q1191" t="n">
+        <v>1024</v>
+      </c>
+      <c r="R1191" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Greens (11.6), Gallup (15.6) og Voxmeter (16.6)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -62817,6 +62817,174 @@
         <v>89</v>
       </c>
     </row>
+    <row r="1196">
+      <c r="A1196" t="n">
+        <v>1195</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1196" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1196" t="n">
+        <v>6</v>
+      </c>
+      <c r="E1196" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1196" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="G1196" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="H1196" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="I1196" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J1196" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="K1196" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="L1196" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1196" t="n">
+        <v>17</v>
+      </c>
+      <c r="N1196" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="O1196" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="P1196" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="Q1196" t="n">
+        <v>1135</v>
+      </c>
+      <c r="R1196" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="n">
+        <v>1196</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1197" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1197" t="n">
+        <v>6</v>
+      </c>
+      <c r="E1197" t="n">
+        <v>15</v>
+      </c>
+      <c r="F1197" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="G1197" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="H1197" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="I1197" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J1197" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="K1197" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="L1197" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M1197" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="N1197" t="n">
+        <v>21</v>
+      </c>
+      <c r="O1197" t="n">
+        <v>9.3</v>
+      </c>
+      <c r="P1197" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="Q1197" t="n">
+        <v>1485</v>
+      </c>
+      <c r="R1197" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="n">
+        <v>1197</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1198" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1198" t="n">
+        <v>6</v>
+      </c>
+      <c r="E1198" t="n">
+        <v>16</v>
+      </c>
+      <c r="F1198" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="G1198" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="H1198" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I1198" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1198" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="K1198" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L1198" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M1198" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="N1198" t="n">
+        <v>19.9</v>
+      </c>
+      <c r="O1198" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="P1198" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Q1198" t="n">
+        <v>1026</v>
+      </c>
+      <c r="R1198" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj YouGov (24.6) og YouGov (8.7)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -379,6 +379,9 @@
   <si>
     <t xml:space="preserve">https://www.dr.dk/nyheder/politik/ny-maaling-alternativets-mandater-bliver-tungen-paa-vaegtskaalen</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://www.bt.dk/politik/blaa-blok-tager-foeringen-men-trekantsdrama-truer</t>
+  </si>
 </sst>
 </file>
 
@@ -63271,6 +63274,118 @@
         <v>89</v>
       </c>
     </row>
+    <row r="1204">
+      <c r="A1204" t="n">
+        <v>1203</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1204" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1204" t="n">
+        <v>6</v>
+      </c>
+      <c r="E1204" t="n">
+        <v>24</v>
+      </c>
+      <c r="F1204" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="G1204" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="H1204" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I1204" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J1204" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K1204" t="n">
+        <v>5</v>
+      </c>
+      <c r="L1204" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M1204" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="N1204" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="O1204" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="P1204" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="Q1204" t="n">
+        <v>1604</v>
+      </c>
+      <c r="R1204" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="n">
+        <v>1204</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1205" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1205" t="n">
+        <v>7</v>
+      </c>
+      <c r="E1205" t="n">
+        <v>8</v>
+      </c>
+      <c r="F1205" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="G1205" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1205" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="I1205" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="J1205" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="K1205" t="n">
+        <v>5</v>
+      </c>
+      <c r="L1205" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M1205" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="N1205" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="O1205" t="n">
+        <v>9.3</v>
+      </c>
+      <c r="P1205" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="Q1205" t="n">
+        <v>1594</v>
+      </c>
+      <c r="R1205" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Greens (2.8) og Voxmeter (5.8)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -382,6 +382,12 @@
   <si>
     <t xml:space="preserve">https://www.bt.dk/politik/blaa-blok-tager-foeringen-men-trekantsdrama-truer</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://twitter.com/hansersej/status/1026575535898611712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://voxmeter.dk/meningsmalinger/</t>
+  </si>
 </sst>
 </file>
 
@@ -63386,6 +63392,118 @@
         <v>122</v>
       </c>
     </row>
+    <row r="1206">
+      <c r="A1206" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1206" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1206" t="n">
+        <v>8</v>
+      </c>
+      <c r="E1206" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1206" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="G1206" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H1206" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="I1206" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="J1206" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K1206" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="L1206" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="M1206" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="N1206" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="O1206" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="P1206" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="Q1206" t="n">
+        <v>1131</v>
+      </c>
+      <c r="R1206" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="n">
+        <v>1206</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1207" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1207" t="n">
+        <v>8</v>
+      </c>
+      <c r="E1207" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1207" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="G1207" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1207" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I1207" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1207" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="K1207" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="L1207" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M1207" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="N1207" t="n">
+        <v>19.9</v>
+      </c>
+      <c r="O1207" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="P1207" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Q1207" t="n">
+        <v>1023</v>
+      </c>
+      <c r="R1207" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tilføj Greens (1.10) og Voxmeter (6.10)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -400,6 +400,9 @@
   <si>
     <t xml:space="preserve">https://politiken.dk/indland/art6729843/%C2%BBVi-er-den-kile-der-lige-nu-borer-sig-ind-i-det-systemsatte-Danmark%C2%AB</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://borsen.dk/nyheder/politik/meningsmaalinger.html</t>
+  </si>
 </sst>
 </file>
 
@@ -64300,6 +64303,116 @@
         <v>124</v>
       </c>
     </row>
+    <row r="1222">
+      <c r="A1222" t="n">
+        <v>1221</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1222" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1222" t="n">
+        <v>10</v>
+      </c>
+      <c r="E1222" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1222" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="G1222" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1222" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I1222" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J1222" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="K1222" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="L1222" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M1222" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="N1222" t="n">
+        <v>19.6</v>
+      </c>
+      <c r="O1222" t="n">
+        <v>10</v>
+      </c>
+      <c r="P1222" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="Q1222"/>
+      <c r="R1222" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="n">
+        <v>1222</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1223" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1223" t="n">
+        <v>10</v>
+      </c>
+      <c r="E1223" t="n">
+        <v>6</v>
+      </c>
+      <c r="F1223" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="G1223" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="H1223" t="n">
+        <v>4</v>
+      </c>
+      <c r="I1223" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J1223" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="K1223" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="L1223" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="M1223" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="N1223" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="O1223" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="P1223" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="Q1223" t="n">
+        <v>1025</v>
+      </c>
+      <c r="R1223" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
opdater stikprøvestørrelsen for Greens (1.10)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -64352,7 +64352,9 @@
       <c r="P1222" t="n">
         <v>3.9</v>
       </c>
-      <c r="Q1222"/>
+      <c r="Q1222" t="n">
+        <v>1157</v>
+      </c>
       <c r="R1222" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
tilføj Norstat (9.10) og Gallup (11.10)
</commit_message>
<xml_diff>
--- a/polls.xlsx
+++ b/polls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -403,6 +403,12 @@
   <si>
     <t xml:space="preserve">https://borsen.dk/nyheder/politik/meningsmaalinger.html</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://www.avisen.dk/meningsmaaling-procentvist-flertal-til-roed-blok_520442.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.berlingske.dk/barometeret</t>
+  </si>
 </sst>
 </file>
 
@@ -64415,6 +64421,118 @@
         <v>124</v>
       </c>
     </row>
+    <row r="1224">
+      <c r="A1224" t="n">
+        <v>1223</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1224" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1224" t="n">
+        <v>10</v>
+      </c>
+      <c r="E1224" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1224" t="n">
+        <v>27.2</v>
+      </c>
+      <c r="G1224" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="H1224" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I1224" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J1224" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="K1224" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="L1224" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M1224" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="N1224" t="n">
+        <v>19</v>
+      </c>
+      <c r="O1224" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="P1224" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="Q1224" t="n">
+        <v>1209</v>
+      </c>
+      <c r="R1224" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="n">
+        <v>1224</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1225" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D1225" t="n">
+        <v>10</v>
+      </c>
+      <c r="E1225" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1225" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="G1225" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="H1225" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I1225" t="n">
+        <v>2</v>
+      </c>
+      <c r="J1225" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="K1225" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="L1225" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M1225" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="N1225" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="O1225" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="P1225" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="Q1225" t="n">
+        <v>1674</v>
+      </c>
+      <c r="R1225" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>